<commit_message>
continued visualisations of annotated data results
</commit_message>
<xml_diff>
--- a/data/ReferenceErrorDetection_data_annotated.xlsx
+++ b/data/ReferenceErrorDetection_data_annotated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b78b8e360351019/_Dokumente/Studium/Master/Masterarbeit/_citation-verification/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Masterarbeit\citation-verification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{3116C6D1-F27C-470A-AF2E-60743673968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A12A4AF5-81B4-4810-A249-BADE86843032}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C74259B-E541-49C6-92FD-3E8C145AE8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="6880" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6242,8 +6242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X254"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>